<commit_message>
Refactor AHP_1_Participant and AHP_Consolidated functions to comment out plotting code; update participant count to 10 and add new participant data files
</commit_message>
<xml_diff>
--- a/AHP/ahp2.xlsx
+++ b/AHP/ahp2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\TUD\DSE\AHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\TUD\DSE\Ekranoplan-DSE\AHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822A8E9C-0EBB-42F6-8170-383DCBB0ACC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9906906-F715-476E-8AEB-F4F9B36B1CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{94C62CCA-CA46-4362-8D9B-A7BDF927CB06}"/>
   </bookViews>
@@ -135,55 +135,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>175524</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>103967</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCECCC70-F86D-37DA-F552-41696CC7609F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5052324" y="106680"/>
-          <a:ext cx="3586043" cy="2743800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,62 +470,62 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>0.16666666666666666</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -585,12 +536,12 @@
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -599,12 +550,12 @@
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -617,7 +568,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>